<commit_message>
xong chức năng Công thức sản xuất
</commit_message>
<xml_diff>
--- a/public/mau-excel/SanPham.xlsx
+++ b/public/mau-excel/SanPham.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\laragon\www\ims\public\mau-excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\ims\public\mau-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DFC00AFB-8EBD-49A0-AE57-1C169A0F8EC8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF0DB8D-3478-452E-80FA-E507C2EC8917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Ảnh sản phẩm</t>
   </si>
@@ -74,6 +74,9 @@
   </si>
   <si>
     <t>Ghi chú</t>
+  </si>
+  <si>
+    <t>Loại sản phẩm (SP_NHA_CUNG_CAP, SP_SAN_XUAT, NGUYEN_LIEU)</t>
   </si>
 </sst>
 </file>
@@ -453,28 +456,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="42.296875" customWidth="1"/>
+    <col min="1" max="1" width="42.25" customWidth="1"/>
     <col min="2" max="2" width="23.5" customWidth="1"/>
-    <col min="3" max="3" width="19.19921875" customWidth="1"/>
+    <col min="3" max="3" width="19.25" customWidth="1"/>
     <col min="4" max="4" width="52.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="59.296875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="63.296875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.796875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.09765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.296875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.625" customWidth="1"/>
+    <col min="6" max="6" width="59.25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.75" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -488,31 +492,34 @@
         <v>13</v>
       </c>
       <c r="E1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" t="s">
         <v>14</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>15</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -525,25 +532,26 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>16</v>
-      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2">
         <v>10000</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>11</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>12</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>20</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
xong chức năng Phiếu xuất kho nguyên liệu sản xuất
</commit_message>
<xml_diff>
--- a/public/mau-excel/SanPham.xlsx
+++ b/public/mau-excel/SanPham.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\laragon\www\ims\public\mau-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9EF0DB8D-3478-452E-80FA-E507C2EC8917}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FD7CF7B-164A-4ED6-B1AD-47948A303B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>Ảnh sản phẩm</t>
   </si>
@@ -55,12 +55,6 @@
     <t>Bánh gạo ABC</t>
   </si>
   <si>
-    <t>5.00</t>
-  </si>
-  <si>
-    <t>10.00</t>
-  </si>
-  <si>
     <t>Danh mục (chọn 1 id trong sheet Danh Mục Sản Phẩm, vd: 1)</t>
   </si>
   <si>
@@ -77,6 +71,9 @@
   </si>
   <si>
     <t>Loại sản phẩm (SP_NHA_CUNG_CAP, SP_SAN_XUAT, NGUYEN_LIEU)</t>
+  </si>
+  <si>
+    <t>SP_NHA_CUNG_CAP</t>
   </si>
 </sst>
 </file>
@@ -458,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -489,16 +486,16 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" t="s">
-        <v>15</v>
       </c>
       <c r="H1" t="s">
         <v>3</v>
@@ -516,7 +513,7 @@
         <v>7</v>
       </c>
       <c r="M1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -532,21 +529,23 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="1"/>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
       <c r="F2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H2">
         <v>10000</v>
       </c>
-      <c r="I2" t="s">
-        <v>11</v>
-      </c>
-      <c r="J2" t="s">
-        <v>12</v>
+      <c r="I2">
+        <v>5</v>
+      </c>
+      <c r="J2">
+        <v>10</v>
       </c>
       <c r="K2">
         <v>20</v>

</xml_diff>